<commit_message>
new changes as: seprate file for reading sheet 2 as value 2 and new function in hb1 for lead creation page 2
</commit_message>
<xml_diff>
--- a/Data/Datss.xlsx
+++ b/Data/Datss.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokesh.Khati\eclipse-workspace\TataAiaAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE2DE8E-B4F3-410B-9AAF-437D602A6C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE0D3A-BD03-496A-ABB4-EE03FE3C3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -70,6 +71,21 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>add1</t>
+  </si>
+  <si>
+    <t>add2</t>
+  </si>
+  <si>
+    <t>landmark</t>
+  </si>
+  <si>
+    <t>qeqw</t>
+  </si>
+  <si>
+    <t>zxczxc</t>
   </si>
 </sst>
 </file>
@@ -79,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +107,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,11 +141,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -493,4 +518,41 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580F5867-1F84-4D05-9787-40B75FED34C3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SIS Personal Page & ProductDashboard changes
</commit_message>
<xml_diff>
--- a/Data/Datss.xlsx
+++ b/Data/Datss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokesh.Khati\eclipse-workspace\TataAiaAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE0D3A-BD03-496A-ABB4-EE03FE3C3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E9FF9-E31F-4B5A-BB18-96ABEA2C6894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>FirstName</t>
   </si>
@@ -86,6 +86,57 @@
   </si>
   <si>
     <t>zxczxc</t>
+  </si>
+  <si>
+    <t>add3</t>
+  </si>
+  <si>
+    <t>heritage</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>sai public school</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>Salaried</t>
+  </si>
+  <si>
+    <t>Age proof</t>
+  </si>
+  <si>
+    <t>HighestEducation</t>
+  </si>
+  <si>
+    <t>Annual Income</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Nominee</t>
+  </si>
+  <si>
+    <t>relation with nominee</t>
+  </si>
+  <si>
+    <t>PAN Card</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>BUXPG1749Q</t>
+  </si>
+  <si>
+    <t>AAC</t>
+  </si>
+  <si>
+    <t>Brother</t>
   </si>
 </sst>
 </file>
@@ -428,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,9 +495,10 @@
     <col min="7" max="7" width="19.21875" customWidth="1"/>
     <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +526,38 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -503,14 +585,44 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2">
+        <v>1500000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="755" yWindow="348" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cities" sqref="F2" xr:uid="{1FD1CF16-C438-4171-B4FA-1DB72FE81F60}">
-      <formula1>$Y$2:$Y$2</formula1>
+      <formula1>$X$2:$X$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -524,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580F5867-1F84-4D05-9787-40B75FED34C3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated data sheet and code of further pages
</commit_message>
<xml_diff>
--- a/Data/Datss.xlsx
+++ b/Data/Datss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokesh.Khati\eclipse-workspace\TataAiaAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E9FF9-E31F-4B5A-BB18-96ABEA2C6894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC9F922-FE9B-4AB9-B3BC-387A6026D4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>FirstName</t>
   </si>
@@ -137,6 +137,57 @@
   </si>
   <si>
     <t>Brother</t>
+  </si>
+  <si>
+    <t>ifsc</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>relType</t>
+  </si>
+  <si>
+    <t>hdfc0001111</t>
+  </si>
+  <si>
+    <t>hdfc</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>fathername</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>motherName</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>wieght</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3I INFOTECH </t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>natureOfWork</t>
+  </si>
+  <si>
+    <t>Web Developers</t>
+  </si>
+  <si>
+    <t>dobb</t>
   </si>
 </sst>
 </file>
@@ -192,12 +243,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,9 +551,15 @@
     <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" customWidth="1"/>
+    <col min="23" max="23" width="21.21875" customWidth="1"/>
+    <col min="27" max="27" width="17.109375" customWidth="1"/>
+    <col min="28" max="28" width="23.77734375" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +617,38 @@
       <c r="S1" t="s">
         <v>31</v>
       </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -615,8 +706,35 @@
       <c r="S2" t="s">
         <v>36</v>
       </c>
+      <c r="T2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" s="5">
+        <v>89674523456789</v>
+      </c>
       <c r="X2" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2">
+        <v>56</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>36212</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +755,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>